<commit_message>
Added one test case Notepad_TC03_replaceText
</commit_message>
<xml_diff>
--- a/InputFiles/Notepad.xlsx
+++ b/InputFiles/Notepad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sakshathtech-my.sharepoint.com/personal/sharika_nambudiri_sakshath-technologies_com/Documents/Desktop/Projects/TestFiles_Katalon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharika\git\Katalon_DesktopAppDemoProject\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_F25DC773A252ABDACC104866291942105BDE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C17FC85-C1A2-4CC2-AF95-BFDF7C6C8E1F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A84ABD-9795-4C6A-9E0B-FC8B322DC452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Text</t>
   </si>
@@ -33,16 +33,28 @@
     <t>FileName</t>
   </si>
   <si>
-    <t>Hii..Welcome to my first desktop project..!!!</t>
-  </si>
-  <si>
     <t>NotepadFile2</t>
   </si>
   <si>
-    <t>Hii..Nice to meet you.!!!</t>
-  </si>
-  <si>
     <t>NotepadFile3</t>
+  </si>
+  <si>
+    <t>NotepadFile4</t>
+  </si>
+  <si>
+    <t>NewText</t>
+  </si>
+  <si>
+    <t>You are enough just as you are!!!</t>
+  </si>
+  <si>
+    <t>Trust the magic of new beginnings!!!</t>
+  </si>
+  <si>
+    <t>Keep going..!!!</t>
+  </si>
+  <si>
+    <t>Good Things take time!!!!</t>
   </si>
 </sst>
 </file>
@@ -101,10 +113,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -382,28 +390,42 @@
     <col min="3" max="3" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>